<commit_message>
Añadida lista de tareas al XLS de historias
</commit_message>
<xml_diff>
--- a/Historias.xlsx
+++ b/Historias.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="10335" windowHeight="5835"/>
+    <workbookView xWindow="600" yWindow="60" windowWidth="10335" windowHeight="5835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Historia</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Identificar a cada jugador</t>
   </si>
   <si>
-    <t>Secuenciar las jugadas</t>
-  </si>
-  <si>
     <t>Barajar</t>
   </si>
   <si>
@@ -75,12 +72,6 @@
     <t>Llevar un conteo de los puntos y juegos que lleva cada pareja</t>
   </si>
   <si>
-    <t>Iniciar una partida</t>
-  </si>
-  <si>
-    <t>Comprobar quién gana una apuesta</t>
-  </si>
-  <si>
     <t>Darse mus</t>
   </si>
   <si>
@@ -96,20 +87,86 @@
     <t>Hacer señas</t>
   </si>
   <si>
-    <t>Controlar las apuestas</t>
-  </si>
-  <si>
     <t>Órdago</t>
   </si>
   <si>
     <t>Conteo de piedras apostadas a cada lance (G,C,P,J/P)</t>
+  </si>
+  <si>
+    <t>Evaluar las piedras que otorga la jugada de un jugador</t>
+  </si>
+  <si>
+    <t>Iniciar una partida (Y pintar la mesa en sus 4 posiciones)</t>
+  </si>
+  <si>
+    <t>Comprobar si un jugador tiene juego y qué pares tiene</t>
+  </si>
+  <si>
+    <t>Pillar una seña</t>
+  </si>
+  <si>
+    <t>Cambiar de pareja</t>
+  </si>
+  <si>
+    <t>Secuenciar los lances</t>
+  </si>
+  <si>
+    <t>Comprobar quién gana un lance</t>
+  </si>
+  <si>
+    <t>Crear un mazo</t>
+  </si>
+  <si>
+    <t>Crear Jugadores</t>
+  </si>
+  <si>
+    <t>Repartir n a un jugador j (Croupier)</t>
+  </si>
+  <si>
+    <t>Crear partida</t>
+  </si>
+  <si>
+    <t>Atributo mano</t>
+  </si>
+  <si>
+    <t>Cambiar mano</t>
+  </si>
+  <si>
+    <t>Crear pareja</t>
+  </si>
+  <si>
+    <t>atributo piedras</t>
+  </si>
+  <si>
+    <t>atributo juegos</t>
+  </si>
+  <si>
+    <t>sumar piedras</t>
+  </si>
+  <si>
+    <t>ganar juego</t>
+  </si>
+  <si>
+    <t>nuevo juego</t>
+  </si>
+  <si>
+    <t>barajar cartas</t>
+  </si>
+  <si>
+    <t>bd cartas</t>
+  </si>
+  <si>
+    <t>dao cartas</t>
+  </si>
+  <si>
+    <t>crear carta/palo/pito/gocho</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,8 +174,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,8 +196,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -155,16 +226,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,9 +555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -493,25 +587,26 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2">
+      <c r="A2" s="5">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>9</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>3</v>
       </c>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>9</v>
@@ -524,8 +619,8 @@
       <c r="A4">
         <v>15</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>20</v>
+      <c r="B4" t="s">
+        <v>31</v>
       </c>
       <c r="C4">
         <v>9</v>
@@ -567,7 +662,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -581,7 +676,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -595,7 +690,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -609,10 +704,13 @@
         <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>8</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -625,183 +723,243 @@
       <c r="C11">
         <v>7</v>
       </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12">
+      <c r="A12" s="5">
         <v>4</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>7</v>
       </c>
+      <c r="D12" s="5">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13">
+      <c r="A13" s="5">
         <v>6</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="5">
         <v>7</v>
       </c>
+      <c r="D13" s="5">
+        <v>3</v>
+      </c>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14">
+      <c r="A14" s="5">
         <v>9</v>
       </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5">
         <v>7</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <v>5</v>
       </c>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>7</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>19</v>
+      <c r="B16" t="s">
+        <v>26</v>
       </c>
       <c r="C16">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>18</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>19</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21">
         <v>7</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>6</v>
+      </c>
+      <c r="D22" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
         <v>12</v>
       </c>
-      <c r="C20">
+      <c r="C23">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21">
+      <c r="B24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="B25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="B26" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -838,7 +996,7 @@
     </row>
   </sheetData>
   <sortState ref="A2:E38">
-    <sortCondition descending="1" ref="C2"/>
+    <sortCondition descending="1" ref="C24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -847,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -860,7 +1018,7 @@
     <col min="3" max="3" width="54.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -874,181 +1032,258 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
+    <row r="2" spans="1:5">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <f t="shared" ref="A3:A30" si="0">A2+1</f>
+      <c r="B2" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <f t="shared" si="0"/>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="7">
+        <v>13</v>
+      </c>
+      <c r="B3" s="7">
+        <v>9</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="8">
+        <v>14</v>
+      </c>
+      <c r="B4" s="8">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <f t="shared" si="0"/>
+      <c r="B7" s="8">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <f t="shared" si="0"/>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <f t="shared" si="0"/>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <f t="shared" si="0"/>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <f t="shared" si="0"/>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <f t="shared" si="0"/>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <f t="shared" si="0"/>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <f t="shared" si="0"/>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="8">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="B15" s="8">
+        <v>6</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17">
-        <f t="shared" si="0"/>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="8">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" s="8">
+        <v>9</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
-        <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:4">
       <c r="A19">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:4">
       <c r="A20">
-        <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:4">
       <c r="A21">
-        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:4">
       <c r="A22">
-        <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:4">
       <c r="A23">
-        <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:4">
       <c r="A24">
-        <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:4">
       <c r="A25">
-        <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:4">
       <c r="A26">
-        <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:4">
       <c r="A27">
-        <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:4">
       <c r="A28">
-        <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:4">
       <c r="A29">
-        <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:4">
       <c r="A30">
-        <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Reordenadas las tareas de la Fase I
</commit_message>
<xml_diff>
--- a/Historias.xlsx
+++ b/Historias.xlsx
@@ -1008,7 +1008,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1081,38 +1081,38 @@
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
-      </c>
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="8">
-        <v>3</v>
-      </c>
-      <c r="B7" s="8">
-        <v>2</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5">

</xml_diff>

<commit_message>
Actualizadas historias de usuario a Lunes 8 14:00
</commit_message>
<xml_diff>
--- a/Historias.xlsx
+++ b/Historias.xlsx
@@ -166,7 +166,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +181,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1008,7 +1013,8 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1100,9 +1106,10 @@
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
@@ -1111,9 +1118,10 @@
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>38</v>
       </c>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
@@ -1122,9 +1130,10 @@
       <c r="B9">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
@@ -1133,9 +1142,10 @@
       <c r="B10">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
@@ -1144,9 +1154,10 @@
       <c r="B11">
         <v>6</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>39</v>
       </c>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
@@ -1155,9 +1166,10 @@
       <c r="B12">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>40</v>
       </c>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
@@ -1166,9 +1178,10 @@
       <c r="B13">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
@@ -1177,9 +1190,10 @@
       <c r="B14">
         <v>6</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="8">
@@ -1200,9 +1214,10 @@
       <c r="B16">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="6" t="s">
         <v>45</v>
       </c>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="8">
@@ -1284,6 +1299,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Cambios para controlar que devuelva NULL el sacar carta cuando se haya quedado sin cartas. Se agregan Test sobre la clase Mazo
</commit_message>
<xml_diff>
--- a/Historias.xlsx
+++ b/Historias.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="10335" windowHeight="5835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="10935" windowHeight="4830"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:D14"/>
 </workbook>
 </file>
 
@@ -560,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -1012,7 +1013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>

</xml_diff>

<commit_message>
Actualziadas Historias 10 Sept
</commit_message>
<xml_diff>
--- a/Historias.xlsx
+++ b/Historias.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="10335" windowHeight="5835" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="60" windowWidth="10335" windowHeight="5835"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t>Historia</t>
   </si>
@@ -160,6 +160,45 @@
   </si>
   <si>
     <t>crear carta/palo/pito/gocho</t>
+  </si>
+  <si>
+    <t>Conteo de piedras apostadas a Grande</t>
+  </si>
+  <si>
+    <t>Conteo de piedras apostadas a Chica</t>
+  </si>
+  <si>
+    <t>Conteo de piedras apostadas a Pares</t>
+  </si>
+  <si>
+    <t>Conteo de piedras apostadas a Juego</t>
+  </si>
+  <si>
+    <t>Conteo de piedras apostadas a Punto</t>
+  </si>
+  <si>
+    <t>Comprobar quién gana a Grande</t>
+  </si>
+  <si>
+    <t>Comprobar quién gana a Chica</t>
+  </si>
+  <si>
+    <t>Comprobar quién gana a Pares</t>
+  </si>
+  <si>
+    <t>Comprobar quién gana a Juego</t>
+  </si>
+  <si>
+    <t>Comprobar quién gana a Punto</t>
+  </si>
+  <si>
+    <t>Interfaz comprobación (comprobar juego, comprobar pares)</t>
+  </si>
+  <si>
+    <t>Enumerado Pares (NO, PAR, MEDIAS, DUPLES)</t>
+  </si>
+  <si>
+    <t>Gestor que lo implemente</t>
   </si>
 </sst>
 </file>
@@ -253,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -264,6 +303,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,9 +601,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -621,18 +662,19 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4">
+      <c r="A4" s="5">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>9</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>13</v>
       </c>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -691,18 +733,19 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9">
+      <c r="A9" s="5">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>8</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>5</v>
       </c>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
@@ -778,18 +821,19 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15">
+      <c r="A15" s="5">
         <v>10</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>7</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <v>5</v>
       </c>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
@@ -805,7 +849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>17</v>
       </c>
@@ -819,7 +863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>18</v>
       </c>
@@ -833,7 +877,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>19</v>
       </c>
@@ -847,21 +891,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
+    <row r="20" spans="1:5">
+      <c r="A20" s="5">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="5">
         <v>8</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>23</v>
       </c>
@@ -875,7 +920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>22</v>
       </c>
@@ -889,7 +934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>7</v>
       </c>
@@ -903,7 +948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>20</v>
       </c>
@@ -917,7 +962,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>24</v>
       </c>
@@ -931,7 +976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>25</v>
       </c>
@@ -939,32 +984,32 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1010,16 +1055,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54.5703125" customWidth="1"/>
   </cols>
@@ -1235,66 +1280,962 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18" s="10">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" s="10">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="B20" s="10">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" s="10">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22">
+      <c r="A22" s="8">
         <v>21</v>
       </c>
+      <c r="B22" s="11">
+        <v>13</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23" s="10">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24" s="10">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" s="10">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26" s="10">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27">
+      <c r="A27" s="8">
         <v>26</v>
       </c>
+      <c r="B27" s="11">
+        <v>15</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" s="10">
+        <v>21</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" s="10">
+        <v>21</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30">
+      <c r="A30" s="8">
         <v>29</v>
       </c>
+      <c r="B30" s="11">
+        <v>21</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="D41" s="7"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="D42" s="7"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="D47" s="7"/>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="D49" s="7"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="D50" s="7"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="D54" s="7"/>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="D55" s="7"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="D56" s="7"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="D58" s="7"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="D59" s="7"/>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="D60" s="7"/>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="D61" s="7"/>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="D62" s="7"/>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="D63" s="7"/>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="D65" s="7"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="D66" s="7"/>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="D67" s="7"/>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="D68" s="7"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="D69" s="7"/>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="D70" s="7"/>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="D71" s="7"/>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="D72" s="7"/>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="D73" s="7"/>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="D74" s="7"/>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="D75" s="7"/>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="D76" s="7"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="D77" s="7"/>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="D78" s="7"/>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="D79" s="7"/>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="D80" s="7"/>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="D81" s="7"/>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="D82" s="7"/>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="D83" s="7"/>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="D84" s="7"/>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="D85" s="7"/>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="D86" s="7"/>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="D87" s="7"/>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="D88" s="7"/>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="D89" s="7"/>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="D90" s="7"/>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="D91" s="7"/>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="D92" s="7"/>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="D93" s="7"/>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="D94" s="7"/>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="D95" s="7"/>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="D96" s="7"/>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="D97" s="7"/>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="D98" s="7"/>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="D99" s="7"/>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="D100" s="7"/>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="D101" s="7"/>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="D102" s="7"/>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="D103" s="7"/>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="D104" s="7"/>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="D105" s="7"/>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="D106" s="7"/>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="D107" s="7"/>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="D108" s="7"/>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="D109" s="7"/>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="D110" s="7"/>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="D111" s="7"/>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="D112" s="7"/>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="D113" s="7"/>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="D114" s="7"/>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="D115" s="7"/>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="D116" s="7"/>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="D117" s="7"/>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="D118" s="7"/>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="D119" s="7"/>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="D120" s="7"/>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="D121" s="7"/>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="D122" s="7"/>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="D123" s="7"/>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="D124" s="7"/>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="D125" s="7"/>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="D126" s="7"/>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="D127" s="7"/>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="D128" s="7"/>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="D129" s="7"/>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="D130" s="7"/>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="D131" s="7"/>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="D132" s="7"/>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="D133" s="7"/>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="D134" s="7"/>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="D135" s="7"/>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="D136" s="7"/>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="D137" s="7"/>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="D138" s="7"/>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="D139" s="7"/>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="D140" s="7"/>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="D141" s="7"/>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="D142" s="7"/>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="D143" s="7"/>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="D144" s="7"/>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="D145" s="7"/>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="D146" s="7"/>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="D147" s="7"/>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="D148" s="7"/>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="D149" s="7"/>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="D150" s="7"/>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="D151" s="7"/>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="D152" s="7"/>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="D153" s="7"/>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="D154" s="7"/>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="D155" s="7"/>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="D156" s="7"/>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="D157" s="7"/>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="D158" s="7"/>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="D159" s="7"/>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="D160" s="7"/>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="D161" s="7"/>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="D162" s="7"/>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="D163" s="7"/>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="D164" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Configurado proyecto mus-servicios como proyecto Web
</commit_message>
<xml_diff>
--- a/Historias.xlsx
+++ b/Historias.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>Historia</t>
   </si>
@@ -199,6 +199,27 @@
   </si>
   <si>
     <t>Gestor que lo implemente</t>
+  </si>
+  <si>
+    <t>Pantalla inicial (y que los jugadores se sienten)</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Checkear los tests</t>
+  </si>
+  <si>
+    <t>Añadir tests faltantes</t>
+  </si>
+  <si>
+    <t>Verificar asertos</t>
+  </si>
+  <si>
+    <t>Poblar BD (Mazo 8/8, 4/4, 0/0)</t>
+  </si>
+  <si>
+    <t>Intefaz de conteo</t>
   </si>
 </sst>
 </file>
@@ -227,7 +248,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +264,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -305,6 +338,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,9 +637,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -662,19 +698,19 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="5">
+      <c r="A4" s="12">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="12">
         <v>9</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="12">
         <v>13</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -836,18 +872,19 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16">
+      <c r="A16" s="13">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="13">
         <v>7</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="13">
         <v>13</v>
       </c>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
@@ -907,18 +944,19 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21">
+      <c r="A21" s="13">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="13">
         <v>7</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="13">
         <v>3</v>
       </c>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
@@ -985,14 +1023,26 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27">
+      <c r="A27" s="13">
         <v>26</v>
       </c>
+      <c r="B27" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28">
+      <c r="A28" s="13">
         <v>27</v>
       </c>
+      <c r="B28" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
@@ -1058,8 +1108,8 @@
   <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1436,43 +1486,79 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="10"/>
+      <c r="B31" s="10">
+        <v>27</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
+      <c r="B32" s="10">
+        <v>27</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
         <v>32</v>
       </c>
+      <c r="B33" s="10">
+        <v>27</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34">
+      <c r="A34" s="8">
         <v>33</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="B34" s="11">
+        <v>27</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="8"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="B35" s="10">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>67</v>
+      </c>
       <c r="D35" s="7"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
         <v>35</v>
       </c>
+      <c r="B36" s="10">
+        <v>23</v>
+      </c>
+      <c r="C36" t="s">
+        <v>60</v>
+      </c>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
         <v>36</v>
       </c>
+      <c r="B37" s="10"/>
       <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4">

</xml_diff>

<commit_message>
Actualizadas historias a 12/09
</commit_message>
<xml_diff>
--- a/Historias.xlsx
+++ b/Historias.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>Historia</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Gestor que lo implemente</t>
+  </si>
+  <si>
+    <t>Pantalla inicial (y que los jugadores se sienten)</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -227,7 +233,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +249,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -305,6 +323,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,9 +622,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -662,19 +683,19 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="5">
+      <c r="A4" s="12">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="12">
         <v>9</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="12">
         <v>13</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -836,18 +857,19 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16">
+      <c r="A16" s="13">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="13">
         <v>7</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="13">
         <v>13</v>
       </c>
+      <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
@@ -907,18 +929,19 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21">
+      <c r="A21" s="13">
         <v>23</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="13">
         <v>7</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="13">
         <v>3</v>
       </c>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
@@ -985,14 +1008,26 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27">
+      <c r="A27" s="13">
         <v>26</v>
       </c>
+      <c r="B27" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28">
+      <c r="A28" s="13">
         <v>27</v>
       </c>
+      <c r="B28" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
@@ -1057,7 +1092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E164"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
     </sheetView>

</xml_diff>

<commit_message>
Actualizadas historias a 16/09
Change-Id: I1541c88ba8389f6697d609ac4b637165e43bba56
</commit_message>
<xml_diff>
--- a/Historias.xlsx
+++ b/Historias.xlsx
@@ -260,7 +260,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -324,6 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -624,7 +625,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -669,18 +670,19 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3">
+      <c r="A3" s="14">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="14">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="14">
         <v>20</v>
       </c>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="12">
@@ -698,60 +700,64 @@
       <c r="E4" s="12"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5">
+      <c r="A5" s="14">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="14">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="14">
         <v>3</v>
       </c>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6">
+      <c r="A6" s="14">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="14">
         <v>8</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="14">
         <v>3</v>
       </c>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7">
+      <c r="A7" s="14">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="14">
         <v>8</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="14">
         <v>2</v>
       </c>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8">
+      <c r="A8" s="14">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="14">
         <v>8</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="14">
         <v>1</v>
       </c>
+      <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5">
@@ -769,32 +775,34 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10">
+      <c r="A10" s="14">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="14">
         <v>8</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="14">
         <v>5</v>
       </c>
+      <c r="E10" s="14"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11">
+      <c r="A11" s="14">
         <v>1</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="14">
         <v>7</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="14">
         <v>8</v>
       </c>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="5">
@@ -857,19 +865,19 @@
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="13">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="5">
         <v>7</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="5">
         <v>13</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
@@ -929,47 +937,49 @@
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="13">
+      <c r="A21" s="5">
         <v>23</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="5">
         <v>7</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="5">
         <v>3</v>
       </c>
-      <c r="E21" s="13"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22">
+      <c r="A22" s="14">
         <v>22</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="14">
         <v>6</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="15">
         <v>8</v>
       </c>
+      <c r="E22" s="14"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23">
+      <c r="A23" s="14">
         <v>7</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="14">
         <v>5</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="14">
         <v>2</v>
       </c>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
@@ -1008,26 +1018,26 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="13">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="13">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">

</xml_diff>

<commit_message>
Sincronizado a 18/09 13:20
Change-Id: I4d10ea2f1747640851220d114645a21392d72ee4
</commit_message>
<xml_diff>
--- a/Historias.xlsx
+++ b/Historias.xlsx
@@ -236,7 +236,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,12 +252,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -326,10 +320,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,7 +621,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -673,94 +666,94 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="14">
+      <c r="A3" s="5">
         <v>8</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="5">
         <v>9</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="5">
         <v>20</v>
       </c>
-      <c r="E3" s="14"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="12">
+      <c r="A4" s="5">
         <v>15</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="5">
         <v>9</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="5">
         <v>13</v>
       </c>
-      <c r="E4" s="12"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="14">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="13">
         <v>8</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>3</v>
       </c>
-      <c r="E5" s="14"/>
+      <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="14">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <v>8</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>3</v>
       </c>
-      <c r="E6" s="14"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="14">
+      <c r="A7" s="13">
         <v>11</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <v>8</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>2</v>
       </c>
-      <c r="E7" s="14"/>
+      <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="14">
+      <c r="A8" s="13">
         <v>12</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <v>8</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="13">
         <v>1</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5">
@@ -778,34 +771,34 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="14">
+      <c r="A10" s="13">
         <v>16</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="13">
         <v>8</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>5</v>
       </c>
-      <c r="E10" s="14"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="14">
+      <c r="A11" s="13">
         <v>1</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="13">
         <v>7</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>8</v>
       </c>
-      <c r="E11" s="14"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="5">
@@ -955,34 +948,34 @@
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="14">
+      <c r="A22" s="13">
         <v>22</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="13">
         <v>6</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="14">
         <v>8</v>
       </c>
-      <c r="E22" s="14"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="14">
+      <c r="A23" s="13">
         <v>7</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="13">
         <v>5</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="13">
         <v>2</v>
       </c>
-      <c r="E23" s="14"/>
+      <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
@@ -1024,7 +1017,7 @@
       <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>61</v>
       </c>
       <c r="C27" s="5"/>
@@ -1035,7 +1028,7 @@
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>62</v>
       </c>
       <c r="C28" s="5"/>
@@ -1043,12 +1036,15 @@
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29">
+      <c r="A29" s="13">
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="14" t="s">
         <v>63</v>
       </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">

</xml_diff>

<commit_message>
Limpados warnings y TODO's
Change-Id: I96febf6e32f35cdfee115e3a90cabc083e5ea22a
</commit_message>
<xml_diff>
--- a/Historias.xlsx
+++ b/Historias.xlsx
@@ -236,7 +236,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -258,6 +258,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -323,6 +329,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,7 +629,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -696,64 +704,64 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="13">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="5">
         <v>8</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="13"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="13">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="5">
         <v>8</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="13">
+      <c r="A7" s="5">
         <v>11</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="5">
         <v>8</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="5">
         <v>2</v>
       </c>
-      <c r="E7" s="13"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="13">
+      <c r="A8" s="5">
         <v>12</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="5">
         <v>8</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5">
@@ -876,46 +884,49 @@
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17">
+      <c r="A17" s="5">
         <v>17</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="5">
         <v>7</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="5">
         <v>8</v>
       </c>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18">
+      <c r="A18" s="15">
         <v>18</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="15">
         <v>7</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="15">
         <v>5</v>
       </c>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19">
+      <c r="A19" s="5">
         <v>19</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="5">
         <v>7</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="5">
         <v>5</v>
       </c>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="5">
@@ -948,34 +959,34 @@
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="13">
+      <c r="A22" s="5">
         <v>22</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="5">
         <v>6</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="12">
         <v>8</v>
       </c>
-      <c r="E22" s="13"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="13">
+      <c r="A23" s="5">
         <v>7</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="5">
         <v>5</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="5">
         <v>2</v>
       </c>
-      <c r="E23" s="13"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">

</xml_diff>